<commit_message>
Finish minimal PRIDE templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/PRIDE/SamplePreparation_PRIDE_minimal.xlsx
+++ b/templates/dataplant/PRIDE/SamplePreparation_PRIDE_minimal.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\dataplant\PRIDE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707E9AC6-FAA8-4E6C-B8E9-A3BEA9AF6CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743727C9-D58F-413B-AEA9-4B8175F6420F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample Preparation" sheetId="1" r:id="rId1"/>
+    <sheet name="SwateTemplateMetadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,20 +36,298 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={A72A4E5C-F5CB-4AF6-9A13-9CEEF48E83E3}</author>
+    <author>tc={C96F1CFD-678D-4452-A3C6-0A624480DE5B}</author>
+    <author>tc={7CAF1F73-B480-4A46-865C-B8B54C01C6B4}</author>
+    <author>tc={F3D3D33A-18F2-4349-A452-44C0AE8C8D9B}</author>
+    <author>tc={DBC66E89-92F1-47CD-ABCB-AD1DDE4F7CD7}</author>
+    <author>tc={84E08C9B-C255-4E5C-B1A5-B95C29D04457}</author>
+    <author>tc={E1C3402D-6F5C-4838-9535-3E60FBBEEC83}</author>
+    <author>tc={732EA3CE-F000-4A14-821B-3B3556E87BF8}</author>
+    <author>tc={4D5F2A55-4BD7-44EA-8C5C-A5DB2B5B7420}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A72A4E5C-F5CB-4AF6-9A13-9CEEF48E83E3}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    The unique identifier of this template. It will be auto generated.
+Antwort:
+    id=09841ab1-ecef-42f3-875f-5810705d191c</t>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="1" shapeId="0" xr:uid="{C96F1CFD-678D-4452-A3C6-0A624480DE5B}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    The name of the Swate template.</t>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="2" shapeId="0" xr:uid="{7CAF1F73-B480-4A46-865C-B8B54C01C6B4}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    The current version of this template in SemVer notation.</t>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="3" shapeId="0" xr:uid="{F3D3D33A-18F2-4349-A452-44C0AE8C8D9B}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    The description of this template. Use few sentences for succinctness.</t>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="4" shapeId="0" xr:uid="{DBC66E89-92F1-47CD-ABCB-AD1DDE4F7CD7}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="5" shapeId="0" xr:uid="{84E08C9B-C255-4E5C-B1A5-B95C29D04457}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    The name of the Swate annotation table in the workbook of the template's excel file.</t>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="6" shapeId="0" xr:uid="{E1C3402D-6F5C-4838-9535-3E60FBBEEC83}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms.</t>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="7" shapeId="0" xr:uid="{732EA3CE-F000-4A14-821B-3B3556E87BF8}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    A list of all tags associated with this template. Tags are realized as Terms.</t>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="8" shapeId="0" xr:uid="{4D5F2A55-4BD7-44EA-8C5C-A5DB2B5B7420}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    The author(s) of this template.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>Source Name</t>
   </si>
   <si>
     <t>Sample Name</t>
+  </si>
+  <si>
+    <t>Parameter [sample processing protocol]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000170)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000170)</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Organisation</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>#ER list</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>ER Term Accession Number</t>
+  </si>
+  <si>
+    <t>ER Term Source REF</t>
+  </si>
+  <si>
+    <t>#TAGS list</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Tags Term Accession Number</t>
+  </si>
+  <si>
+    <t>Tags Term Source REF</t>
+  </si>
+  <si>
+    <t>#AUTHORS list</t>
+  </si>
+  <si>
+    <t>Authors Last Name</t>
+  </si>
+  <si>
+    <t>Authors First Name</t>
+  </si>
+  <si>
+    <t>Authors Mid Initials</t>
+  </si>
+  <si>
+    <t>Authors Email</t>
+  </si>
+  <si>
+    <t>Authors Phone</t>
+  </si>
+  <si>
+    <t>Authors Fax</t>
+  </si>
+  <si>
+    <t>Authors Address</t>
+  </si>
+  <si>
+    <t>Authors Affiliation</t>
+  </si>
+  <si>
+    <t>Authors ORCID</t>
+  </si>
+  <si>
+    <t>Authors Role</t>
+  </si>
+  <si>
+    <t>Authors Role Term Accession Number</t>
+  </si>
+  <si>
+    <t>Authors Role Term Source REF</t>
+  </si>
+  <si>
+    <t>09841ab1-ecef-42f3-875f-5810705d191c</t>
+  </si>
+  <si>
+    <t>Sample Preparation (PRIDE minimal)</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>A template for annotating experimental metadata regarding the preparation of samples for MS measurement, meeting the requirements for PRIDE submission.</t>
+  </si>
+  <si>
+    <t>DataPLANT</t>
+  </si>
+  <si>
+    <t>annotationTableGentleNewt91</t>
+  </si>
+  <si>
+    <t>PRIDE</t>
+  </si>
+  <si>
+    <t>Proteomics</t>
+  </si>
+  <si>
+    <t>Maus</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>maus@nfdi4plants.org</t>
+  </si>
+  <si>
+    <t>Erwin-Schrödinger-Str. 56, 67663 Kaiserslautern</t>
+  </si>
+  <si>
+    <t>CSB, RPTU Kaiserslautern</t>
+  </si>
+  <si>
+    <t>Data-Steward</t>
+  </si>
+  <si>
+    <t>0000-0002-8241-5300</t>
+  </si>
+  <si>
+    <t>Mass spectrometry</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Preparation</t>
+  </si>
+  <si>
+    <t>Characteristic [Organism]</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCIT:C14250)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCIT:C14250)</t>
+  </si>
+  <si>
+    <t>Characteristic [Tissue]</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCIT:C12801)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCIT:C12801)</t>
+  </si>
+  <si>
+    <t>Characteristic [cell type]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000069)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000069)</t>
+  </si>
+  <si>
+    <t>Characteristic [disease]</t>
+  </si>
+  <si>
+    <t>Term Source REF (EFO:0000408)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (EFO:0000408)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,16 +335,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFF5F5F5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF217346"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FCDB3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0E5C2F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC21F3A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -73,17 +398,166 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFEFEFE"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFEFEFE"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFEFEFE"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFEFEFE"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFEFEFE"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFEFEFE"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFEFEFE"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFEFEFE"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -96,11 +570,32 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Oliver Maus" id="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" userId="855bec4539777958" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F8F83614-7641-41C2-A36B-B773352D00E6}" name="annotationTableGentleNewt91" displayName="annotationTableGentleNewt91" ref="A1:B2" totalsRowShown="0">
-  <autoFilter ref="A1:B2" xr:uid="{F8F83614-7641-41C2-A36B-B773352D00E6}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F8F83614-7641-41C2-A36B-B773352D00E6}" name="annotationTableGentleNewt91" displayName="annotationTableGentleNewt91" ref="A1:Q2" totalsRowShown="0">
+  <autoFilter ref="A1:Q2" xr:uid="{F8F83614-7641-41C2-A36B-B773352D00E6}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{EF11BDF6-547C-4BC9-A2EB-4925D2CBE2D9}" name="Source Name"/>
+    <tableColumn id="3" xr3:uid="{1742D588-5279-4B10-988A-1288A7C12E85}" name="Parameter [sample processing protocol]" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{6C410FDA-6F9F-4153-9193-2049E60F28C3}" name="Term Source REF (DPBO:1000170)" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{4FAF3CE3-4A64-4A97-8D05-1AC34C42E601}" name="Term Accession Number (DPBO:1000170)" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{EEF4CF29-6E99-4DB0-B18D-766E93AC2CFF}" name="Characteristic [Organism]" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{8AFA9BF2-82CB-4CC8-8CDD-FF925F826879}" name="Term Source REF (NCIT:C14250)" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{5C348F63-ECCB-4A46-BA99-F421003B91BF}" name="Term Accession Number (NCIT:C14250)" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{3A0520E0-0B32-4762-9CFD-524B62B870BD}" name="Characteristic [Tissue]" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{D27C16CB-2FC4-4658-A154-E1A0343E7919}" name="Term Source REF (NCIT:C12801)" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{EED8D5F7-CAB5-4702-889A-E6D48AFD9F2B}" name="Term Accession Number (NCIT:C12801)" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{E2C318A6-FFD3-445A-B2F6-BE10EB7DA336}" name="Characteristic [cell type]" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{ECF4CDED-AE5B-4408-A56B-732A4F21721E}" name="Term Source REF (DPBO:0000069)" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{BC983C19-0FBD-4294-8BEF-248948D9B5BE}" name="Term Accession Number (DPBO:0000069)" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{D07D02C4-71AD-46DF-BB68-378C6650D24B}" name="Characteristic [disease]" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{ED1669E1-CF24-48A4-BB33-9E865C89537D}" name="Term Source REF (EFO:0000408)" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{AADA719C-77D2-4658-BAC4-67D4130F136B}" name="Term Accession Number (EFO:0000408)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{AB47EA39-A4FC-4419-B215-93863548DC98}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -368,10 +863,48 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2023-08-15T10:23:16.12" personId="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" id="{A72A4E5C-F5CB-4AF6-9A13-9CEEF48E83E3}">
+    <text>The unique identifier of this template. It will be auto generated.</text>
+  </threadedComment>
+  <threadedComment ref="A1" dT="2023-08-15T10:23:16.13" personId="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" id="{CF893BC6-9F47-458F-892F-D582D3E0B014}" parentId="{A72A4E5C-F5CB-4AF6-9A13-9CEEF48E83E3}">
+    <text>id=09841ab1-ecef-42f3-875f-5810705d191c</text>
+  </threadedComment>
+  <threadedComment ref="A2" dT="2023-08-15T10:23:16.13" personId="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" id="{C96F1CFD-678D-4452-A3C6-0A624480DE5B}">
+    <text>The name of the Swate template.</text>
+  </threadedComment>
+  <threadedComment ref="A3" dT="2023-08-15T10:23:16.13" personId="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" id="{7CAF1F73-B480-4A46-865C-B8B54C01C6B4}">
+    <text>The current version of this template in SemVer notation.</text>
+  </threadedComment>
+  <threadedComment ref="A4" dT="2023-08-15T10:23:16.13" personId="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" id="{F3D3D33A-18F2-4349-A452-44C0AE8C8D9B}">
+    <text>The description of this template. Use few sentences for succinctness.</text>
+  </threadedComment>
+  <threadedComment ref="A5" dT="2023-08-15T10:23:16.13" personId="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" id="{DBC66E89-92F1-47CD-ABCB-AD1DDE4F7CD7}">
+    <text>The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</text>
+  </threadedComment>
+  <threadedComment ref="A6" dT="2023-08-15T10:23:16.13" personId="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" id="{84E08C9B-C255-4E5C-B1A5-B95C29D04457}">
+    <text>The name of the Swate annotation table in the workbook of the template's excel file.</text>
+  </threadedComment>
+  <threadedComment ref="A7" dT="2023-08-15T10:23:16.13" personId="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" id="{E1C3402D-6F5C-4838-9535-3E60FBBEEC83}">
+    <text>A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms.</text>
+  </threadedComment>
+  <threadedComment ref="A11" dT="2023-08-15T10:23:16.14" personId="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" id="{732EA3CE-F000-4A14-821B-3B3556E87BF8}">
+    <text>A list of all tags associated with this template. Tags are realized as Terms.</text>
+  </threadedComment>
+  <threadedComment ref="A15" dT="2023-08-15T10:23:16.14" personId="{63FD3E59-8E42-459F-A0D1-F7FA17C9AAE6}" id="{4D5F2A55-4BD7-44EA-8C5C-A5DB2B5B7420}">
+    <text>The author(s) of this template.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="531" row="1">
+  <wetp:taskpane dockstate="right" visibility="0" width="622" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="0" width="575" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
@@ -386,24 +919,142 @@
 </we:webextension>
 </file>
 
+<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{5E5EC249-0954-47A5-B28C-C4D0FC129A09}">
+  <we:reference id="5d6f5462-3401-48ec-9406-d12882e9ad84" version="0.8.0.0" store="\\NB-W-2020-11-OM\nfdi_manifest_olive" storeType="Filesystem"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="38" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="38" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.7109375" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="39.85546875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.140625" customWidth="1"/>
+    <col min="19" max="19" width="38.140625" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -412,4 +1063,268 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA2BE12E-6D0B-49DC-94EF-B51B9DB11569}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="10"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B19" r:id="rId1" xr:uid="{3941365B-374D-47C9-B300-A84C7671E469}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<customXml>
+  <SwateTable Table="annotationTableGentleNewt91">
+    <TableValidation DateTime="2023-08-15 12:21" SwateVersion="0.7.1" TableName="annotationTableGentleNewt91" Userlist="">
+      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="5" Unit="None" ValidationFormat="Text"/>
+      <ColumnValidation ColumnAdress="1" ColumnHeader="Parameter [sample processing protocol]" Importance="5" Unit="None" ValidationFormat="OntologyTerm (sample processing protocol)"/>
+      <ColumnValidation ColumnAdress="4" ColumnHeader="Characteristic [Organism]" Importance="5" Unit="None" ValidationFormat="OntologyTerm Organism"/>
+      <ColumnValidation ColumnAdress="7" ColumnHeader="Characteristic [Tissue]" Importance="5" Unit="None" ValidationFormat="OntologyTerm Tissue"/>
+      <ColumnValidation ColumnAdress="10" ColumnHeader="Characteristic [cell type]" Importance="3" Unit="None" ValidationFormat="OntologyTerm (cell type)"/>
+      <ColumnValidation ColumnAdress="13" ColumnHeader="Characteristic [disease]" Importance="3" Unit="None" ValidationFormat="OntologyTerm disease"/>
+      <ColumnValidation ColumnAdress="16" ColumnHeader="Sample Name" Importance="5" Unit="None" ValidationFormat="Text"/>
+    </TableValidation>
+  </SwateTable>
+</customXml>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21F8A4A7-B7A7-474E-99C1-A549D3C849B0}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
</xml_diff>